<commit_message>
finishing up styling assessments
</commit_message>
<xml_diff>
--- a/LWTasks.xlsx
+++ b/LWTasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austin.wise\Desktop\LandWise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF8C0D8-FF69-4EAD-BB55-5AAD16782AAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439F88F5-0594-4C2F-A318-ADD65C1B41F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3503" yWindow="345" windowWidth="18225" windowHeight="11423" activeTab="2" xr2:uid="{6AADF604-8123-4F92-97E6-F0BFD65D7E5B}"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="18224" windowHeight="11422" xr2:uid="{6AADF604-8123-4F92-97E6-F0BFD65D7E5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Task List" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="108">
   <si>
     <t>Location</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>design and layout (kanban board)</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -940,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A45098-DFA6-4422-8359-F8F72E4491BF}">
   <dimension ref="A2:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -987,7 +990,9 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
@@ -1673,8 +1678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98F05DB-98C4-451B-B919-B88DE96D1CCA}">
   <dimension ref="A2:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>